<commit_message>
updated slide templates + paths
</commit_message>
<xml_diff>
--- a/Datasets/UCD_EngArch_Path_Biomed-Elec_ME_Modules.xlsx
+++ b/Datasets/UCD_EngArch_Path_Biomed-Elec_ME_Modules.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\SATLE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alanh\Documents\GitHub\ChatGPTAssessment\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF53AFED-7D5D-4BF2-B94B-22C43DDDEFBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF4A4801-0BA6-4681-B84A-B75B0AEB6735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C7146B4A-4439-46E0-B60E-DB05B9DBCCC1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="78">
   <si>
     <t>EEEN20020</t>
   </si>
@@ -231,9 +231,6 @@
   </si>
   <si>
     <t>EEEN40010</t>
-  </si>
-  <si>
-    <t>M</t>
   </si>
   <si>
     <t>T160</t>
@@ -633,7 +630,7 @@
   <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29:S50"/>
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1619,11 +1616,11 @@
       <c r="D38">
         <v>4</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38">
+        <v>4</v>
+      </c>
+      <c r="F38" t="s">
         <v>65</v>
-      </c>
-      <c r="F38" t="s">
-        <v>66</v>
       </c>
       <c r="G38">
         <v>5</v>
@@ -1645,11 +1642,11 @@
       <c r="D39">
         <v>4</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39">
+        <v>4</v>
+      </c>
+      <c r="F39" t="s">
         <v>65</v>
-      </c>
-      <c r="F39" t="s">
-        <v>66</v>
       </c>
       <c r="G39">
         <v>5</v>
@@ -1671,11 +1668,11 @@
       <c r="D40">
         <v>4</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40">
+        <v>4</v>
+      </c>
+      <c r="F40" t="s">
         <v>65</v>
-      </c>
-      <c r="F40" t="s">
-        <v>66</v>
       </c>
       <c r="G40">
         <v>5</v>
@@ -1697,11 +1694,11 @@
       <c r="D41">
         <v>4</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41">
+        <v>4</v>
+      </c>
+      <c r="F41" t="s">
         <v>65</v>
-      </c>
-      <c r="F41" t="s">
-        <v>66</v>
       </c>
       <c r="G41">
         <v>5</v>
@@ -1723,11 +1720,11 @@
       <c r="D42">
         <v>4</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42">
+        <v>4</v>
+      </c>
+      <c r="F42" t="s">
         <v>65</v>
-      </c>
-      <c r="F42" t="s">
-        <v>66</v>
       </c>
       <c r="G42">
         <v>5</v>
@@ -1738,7 +1735,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B43" t="s">
         <v>30</v>
@@ -1749,11 +1746,11 @@
       <c r="D43">
         <v>4</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43">
+        <v>4</v>
+      </c>
+      <c r="F43" t="s">
         <v>65</v>
-      </c>
-      <c r="F43" t="s">
-        <v>66</v>
       </c>
       <c r="G43">
         <v>5</v>
@@ -1764,7 +1761,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B44" t="s">
         <v>30</v>
@@ -1775,11 +1772,11 @@
       <c r="D44">
         <v>4</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44">
+        <v>4</v>
+      </c>
+      <c r="F44" t="s">
         <v>65</v>
-      </c>
-      <c r="F44" t="s">
-        <v>66</v>
       </c>
       <c r="G44">
         <v>30</v>
@@ -1790,7 +1787,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B45" t="s">
         <v>30</v>
@@ -1801,11 +1798,11 @@
       <c r="D45">
         <v>4</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E45">
+        <v>5</v>
+      </c>
+      <c r="F45" t="s">
         <v>65</v>
-      </c>
-      <c r="F45" t="s">
-        <v>66</v>
       </c>
       <c r="G45">
         <v>20</v>
@@ -1816,7 +1813,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B46" t="s">
         <v>30</v>
@@ -1827,11 +1824,11 @@
       <c r="D46">
         <v>4</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46">
+        <v>5</v>
+      </c>
+      <c r="F46" t="s">
         <v>65</v>
-      </c>
-      <c r="F46" t="s">
-        <v>66</v>
       </c>
       <c r="G46">
         <v>5</v>
@@ -1842,7 +1839,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B47" t="s">
         <v>30</v>
@@ -1853,11 +1850,11 @@
       <c r="D47">
         <v>4</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47">
+        <v>5</v>
+      </c>
+      <c r="F47" t="s">
         <v>65</v>
-      </c>
-      <c r="F47" t="s">
-        <v>66</v>
       </c>
       <c r="G47">
         <v>5</v>
@@ -1868,7 +1865,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B48" t="s">
         <v>30</v>
@@ -1879,11 +1876,11 @@
       <c r="D48">
         <v>4</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E48">
+        <v>5</v>
+      </c>
+      <c r="F48" t="s">
         <v>65</v>
-      </c>
-      <c r="F48" t="s">
-        <v>66</v>
       </c>
       <c r="G48">
         <v>5</v>
@@ -1894,7 +1891,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B49" t="s">
         <v>30</v>
@@ -1905,11 +1902,11 @@
       <c r="D49">
         <v>4</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E49">
+        <v>5</v>
+      </c>
+      <c r="F49" t="s">
         <v>65</v>
-      </c>
-      <c r="F49" t="s">
-        <v>66</v>
       </c>
       <c r="G49">
         <v>5</v>
@@ -1920,22 +1917,22 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B50" t="s">
         <v>29</v>
       </c>
       <c r="C50" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D50">
         <v>4</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E50">
+        <v>5</v>
+      </c>
+      <c r="F50" t="s">
         <v>65</v>
-      </c>
-      <c r="F50" t="s">
-        <v>66</v>
       </c>
       <c r="G50">
         <v>5</v>
@@ -1946,22 +1943,22 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B51" t="s">
         <v>29</v>
       </c>
       <c r="C51" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D51">
         <v>4</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E51">
+        <v>5</v>
+      </c>
+      <c r="F51" t="s">
         <v>65</v>
-      </c>
-      <c r="F51" t="s">
-        <v>66</v>
       </c>
       <c r="G51">
         <v>5</v>
@@ -1972,7 +1969,7 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B52" t="s">
         <v>30</v>
@@ -1983,11 +1980,11 @@
       <c r="D52">
         <v>4</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52">
+        <v>5</v>
+      </c>
+      <c r="F52" t="s">
         <v>65</v>
-      </c>
-      <c r="F52" t="s">
-        <v>66</v>
       </c>
       <c r="G52">
         <v>5</v>
@@ -1998,7 +1995,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B53" t="s">
         <v>30</v>
@@ -2009,11 +2006,11 @@
       <c r="D53">
         <v>4</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E53">
+        <v>5</v>
+      </c>
+      <c r="F53" t="s">
         <v>65</v>
-      </c>
-      <c r="F53" t="s">
-        <v>66</v>
       </c>
       <c r="G53">
         <v>5</v>

</xml_diff>

<commit_message>
BIOMED + ELECTRONIC + MECH + STRUCT ENG WITH ARCH CHECKED
</commit_message>
<xml_diff>
--- a/Datasets/UCD_EngArch_Path_Biomed-Elec_ME_Modules.xlsx
+++ b/Datasets/UCD_EngArch_Path_Biomed-Elec_ME_Modules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alanh\Documents\GitHub\ChatGPTAssessment\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF4A4801-0BA6-4681-B84A-B75B0AEB6735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B441CF04-F2BF-4E81-81AD-E55F440B014D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C7146B4A-4439-46E0-B60E-DB05B9DBCCC1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="79">
   <si>
     <t>EEEN20020</t>
   </si>
@@ -270,6 +270,9 @@
   </si>
   <si>
     <t>CompSci</t>
+  </si>
+  <si>
+    <t>MEEN30140</t>
   </si>
 </sst>
 </file>
@@ -629,16 +632,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{470AD8BE-D0F1-4863-8083-BF0D6224CD04}">
   <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J35" sqref="A1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="44.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1579,7 +1580,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="B37" t="s">
         <v>30</v>
@@ -1588,7 +1589,7 @@
         <v>28</v>
       </c>
       <c r="D37">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E37">
         <v>3</v>
@@ -1600,7 +1601,7 @@
         <v>5</v>
       </c>
       <c r="H37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>